<commit_message>
Update experimental results for the consistency in evaluation metric term
</commit_message>
<xml_diff>
--- a/experiment_results/SBFL_ONLY/Summary/All/single_bug_rank_exam.xlsx
+++ b/experiment_results/SBFL_ONLY/Summary/All/single_bug_rank_exam.xlsx
@@ -484,7 +484,7 @@
         <v>18.48082595870207</v>
       </c>
       <c r="D2">
-        <v>3.510112814463905</v>
+        <v>3.510112814463906</v>
       </c>
       <c r="E2">
         <v>788.5516224188791</v>
@@ -501,7 +501,7 @@
         <v>14.94100294985251</v>
       </c>
       <c r="D3">
-        <v>2.322804917716258</v>
+        <v>2.322804917716262</v>
       </c>
       <c r="E3">
         <v>788.5516224188791</v>
@@ -535,7 +535,7 @@
         <v>18.48377581120944</v>
       </c>
       <c r="D5">
-        <v>3.513994199342029</v>
+        <v>3.513994199342031</v>
       </c>
       <c r="E5">
         <v>788.5516224188791</v>
@@ -552,7 +552,7 @@
         <v>14.89675516224189</v>
       </c>
       <c r="D6">
-        <v>2.313015116366422</v>
+        <v>2.313015116366424</v>
       </c>
       <c r="E6">
         <v>788.5516224188791</v>
@@ -586,7 +586,7 @@
         <v>292.4129793510324</v>
       </c>
       <c r="D8">
-        <v>36.66744407181165</v>
+        <v>36.66744407181167</v>
       </c>
       <c r="E8">
         <v>788.5516224188791</v>
@@ -603,7 +603,7 @@
         <v>292.4129793510324</v>
       </c>
       <c r="D9">
-        <v>36.66744407181165</v>
+        <v>36.66744407181167</v>
       </c>
       <c r="E9">
         <v>788.5516224188791</v>
@@ -637,7 +637,7 @@
         <v>16.97345132743363</v>
       </c>
       <c r="D11">
-        <v>2.90917753508307</v>
+        <v>2.909177535083074</v>
       </c>
       <c r="E11">
         <v>788.5516224188791</v>
@@ -654,7 +654,7 @@
         <v>17.12979351032448</v>
       </c>
       <c r="D12">
-        <v>2.98387107593841</v>
+        <v>2.983871075938416</v>
       </c>
       <c r="E12">
         <v>788.5516224188791</v>
@@ -671,7 +671,7 @@
         <v>61.49262536873157</v>
       </c>
       <c r="D13">
-        <v>9.902636816512844</v>
+        <v>9.902636816512814</v>
       </c>
       <c r="E13">
         <v>788.5516224188791</v>
@@ -688,7 +688,7 @@
         <v>64.84955752212389</v>
       </c>
       <c r="D14">
-        <v>10.04770735036731</v>
+        <v>10.04770735036728</v>
       </c>
       <c r="E14">
         <v>788.5516224188791</v>
@@ -705,7 +705,7 @@
         <v>15.09439528023599</v>
       </c>
       <c r="D15">
-        <v>2.378060112863562</v>
+        <v>2.378060112863567</v>
       </c>
       <c r="E15">
         <v>788.5516224188791</v>
@@ -722,7 +722,7 @@
         <v>13.6283185840708</v>
       </c>
       <c r="D16">
-        <v>2.102801105200222</v>
+        <v>2.102801105200223</v>
       </c>
       <c r="E16">
         <v>788.5516224188791</v>
@@ -756,7 +756,7 @@
         <v>292.4129793510324</v>
       </c>
       <c r="D18">
-        <v>36.66744407181165</v>
+        <v>36.66744407181167</v>
       </c>
       <c r="E18">
         <v>788.5516224188791</v>
@@ -773,7 +773,7 @@
         <v>16.97345132743363</v>
       </c>
       <c r="D19">
-        <v>2.90917753508307</v>
+        <v>2.909177535083074</v>
       </c>
       <c r="E19">
         <v>788.5516224188791</v>
@@ -790,7 +790,7 @@
         <v>16.97345132743363</v>
       </c>
       <c r="D20">
-        <v>2.90917753508307</v>
+        <v>2.909177535083074</v>
       </c>
       <c r="E20">
         <v>788.5516224188791</v>
@@ -807,7 +807,7 @@
         <v>292.4129793510324</v>
       </c>
       <c r="D21">
-        <v>36.66744407181165</v>
+        <v>36.66744407181167</v>
       </c>
       <c r="E21">
         <v>788.5516224188791</v>
@@ -824,7 +824,7 @@
         <v>292.4129793510324</v>
       </c>
       <c r="D22">
-        <v>36.66744407181165</v>
+        <v>36.66744407181167</v>
       </c>
       <c r="E22">
         <v>788.5516224188791</v>
@@ -841,7 +841,7 @@
         <v>292.4129793510324</v>
       </c>
       <c r="D23">
-        <v>36.66744407181165</v>
+        <v>36.66744407181167</v>
       </c>
       <c r="E23">
         <v>788.5516224188791</v>
@@ -858,7 +858,7 @@
         <v>13.58407079646018</v>
       </c>
       <c r="D24">
-        <v>2.09435192458823</v>
+        <v>2.094351924588231</v>
       </c>
       <c r="E24">
         <v>788.5516224188791</v>
@@ -892,7 +892,7 @@
         <v>292.4129793510324</v>
       </c>
       <c r="D26">
-        <v>36.66744407181165</v>
+        <v>36.66744407181167</v>
       </c>
       <c r="E26">
         <v>788.5516224188791</v>
@@ -909,7 +909,7 @@
         <v>64.72566371681415</v>
       </c>
       <c r="D27">
-        <v>10.60651767402473</v>
+        <v>10.60651767402472</v>
       </c>
       <c r="E27">
         <v>788.5516224188791</v>
@@ -926,7 +926,7 @@
         <v>16.97345132743363</v>
       </c>
       <c r="D28">
-        <v>2.90917753508307</v>
+        <v>2.909177535083074</v>
       </c>
       <c r="E28">
         <v>788.5516224188791</v>
@@ -943,7 +943,7 @@
         <v>13.6165191740413</v>
       </c>
       <c r="D29">
-        <v>2.764107001228604</v>
+        <v>2.764107001228609</v>
       </c>
       <c r="E29">
         <v>788.5516224188791</v>
@@ -977,7 +977,7 @@
         <v>13.88790560471976</v>
       </c>
       <c r="D31">
-        <v>2.117623758423508</v>
+        <v>2.117623758423509</v>
       </c>
       <c r="E31">
         <v>788.5516224188791</v>

</xml_diff>